<commit_message>
updating as another user
</commit_message>
<xml_diff>
--- a/CSD_Daily_status.xlsx
+++ b/CSD_Daily_status.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\bench_status\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PERS\bench_status\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19693529-0DDA-491B-893C-919144799ACA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7324F69D-B78C-483B-A45D-EBD97A433153}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="kWFHmNGnqNKFGijJvfabpUvI1EKsE0VWrBedqe5ViS0byVu+xezzeGL/1vzrR4TYE2jxLdUqJ5l+ZYPmwCdWxg==" workbookSaltValue="C6ZiAuHqpsuNFxKAC/BOLA==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="14" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -711,7 +711,7 @@
     <t>Going through DevOps training</t>
   </si>
   <si>
-    <t>Going through Devops Training - Jenkins pipeline</t>
+    <t>Going through Devops Training - Jenkins pipeline.</t>
   </si>
 </sst>
 </file>
@@ -21076,7 +21076,7 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Added sheet for 21st
</commit_message>
<xml_diff>
--- a/CSD_Daily_status.xlsx
+++ b/CSD_Daily_status.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thejms\bench_status\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\bench_status\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="kWFHmNGnqNKFGijJvfabpUvI1EKsE0VWrBedqe5ViS0byVu+xezzeGL/1vzrR4TYE2jxLdUqJ5l+ZYPmwCdWxg==" workbookSaltValue="C6ZiAuHqpsuNFxKAC/BOLA==" workbookSpinCount="100000" lockStructure="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F604D4B8-9973-4657-B41A-C979ED32F89C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19890" windowHeight="7560" firstSheet="14" activeTab="17"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="15" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="status-18-03-2020" sheetId="14" r:id="rId1"/>
@@ -31,13 +31,14 @@
     <sheet name="Status-10-04-2020" sheetId="32" r:id="rId16"/>
     <sheet name="Status-17-04-2020" sheetId="34" r:id="rId17"/>
     <sheet name="Status-20-04-2020" sheetId="35" r:id="rId18"/>
+    <sheet name="Status-21-04-2020" sheetId="36" r:id="rId19"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="835" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="882" uniqueCount="226">
   <si>
     <t>Date</t>
   </si>
@@ -720,7 +721,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="11">
     <font>
       <sz val="11"/>
@@ -1263,7 +1264,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:XFD29"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
@@ -18008,7 +18010,8 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -18349,7 +18352,8 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+  <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -18696,7 +18700,8 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+  <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -19045,7 +19050,8 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+  <sheetPr codeName="Sheet13"/>
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -19397,7 +19403,8 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+  <sheetPr codeName="Sheet14"/>
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
@@ -19749,7 +19756,8 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+  <sheetPr codeName="Sheet15"/>
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -20101,7 +20109,8 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+  <sheetPr codeName="Sheet16"/>
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
@@ -20453,10 +20462,11 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+  <sheetPr codeName="Sheet17"/>
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -21024,11 +21034,12 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+  <sheetPr codeName="Sheet18"/>
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
@@ -21538,8 +21549,514 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B3C9E85-6CBB-4D80-8E1B-10638ABAC88C}">
+  <sheetPr codeName="Sheet19"/>
+  <dimension ref="A1:F31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="10.453125" customWidth="1"/>
+    <col min="2" max="2" width="16.26953125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="38.26953125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="49.453125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="27.6328125" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4">
+        <v>94597</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="5"/>
+      <c r="E2" s="6">
+        <v>9</v>
+      </c>
+      <c r="F2" s="7"/>
+    </row>
+    <row r="3" spans="1:6" ht="27.5" customHeight="1">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>67908</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="35.5" customHeight="1">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>156137</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="6">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4">
+        <v>189815</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4">
+        <v>119065</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D6" s="8"/>
+      <c r="E6" s="9">
+        <v>9</v>
+      </c>
+      <c r="F6" s="10"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="6">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>185010</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="E7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="6">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>154447</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D8" s="8"/>
+      <c r="E8" s="12">
+        <v>9</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="32.5" customHeight="1">
+      <c r="A9" s="6">
+        <v>8</v>
+      </c>
+      <c r="B9" s="13"/>
+      <c r="C9" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="D9" s="15"/>
+      <c r="E9" s="12">
+        <v>9</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="34" customHeight="1">
+      <c r="A10" s="6">
+        <v>9</v>
+      </c>
+      <c r="B10" s="14">
+        <v>175816</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="D10" s="15"/>
+      <c r="E10" s="16">
+        <v>9</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="6">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4">
+        <v>191221</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="D11" s="18"/>
+      <c r="E11" s="12">
+        <v>9</v>
+      </c>
+      <c r="F11" s="18"/>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="6">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4">
+        <v>46014906</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="D12" s="20"/>
+      <c r="E12" s="12">
+        <v>9</v>
+      </c>
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="6">
+        <v>12</v>
+      </c>
+      <c r="B13" s="20">
+        <v>156635</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>190</v>
+      </c>
+      <c r="D13" s="20"/>
+      <c r="E13" s="12">
+        <v>9</v>
+      </c>
+      <c r="F13" s="7"/>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="6">
+        <v>13</v>
+      </c>
+      <c r="B14" s="20">
+        <v>168293</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>192</v>
+      </c>
+      <c r="E14" s="12">
+        <v>9</v>
+      </c>
+      <c r="F14" s="7"/>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="6">
+        <v>14</v>
+      </c>
+      <c r="B15" s="20">
+        <v>151146</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>194</v>
+      </c>
+      <c r="E15" s="12">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="6">
+        <v>15</v>
+      </c>
+      <c r="B16" s="20">
+        <v>156996</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>195</v>
+      </c>
+      <c r="E16" s="12">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="6">
+        <v>16</v>
+      </c>
+      <c r="B17" s="20">
+        <v>185599</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>196</v>
+      </c>
+      <c r="E17" s="12">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="6">
+        <v>17</v>
+      </c>
+      <c r="B18" s="20">
+        <v>96340</v>
+      </c>
+      <c r="C18" s="20" t="s">
+        <v>198</v>
+      </c>
+      <c r="E18" s="12">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="6">
+        <v>18</v>
+      </c>
+      <c r="B19" s="20">
+        <v>108444</v>
+      </c>
+      <c r="C19" s="20" t="s">
+        <v>199</v>
+      </c>
+      <c r="E19" s="12">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="29">
+      <c r="A20" s="21">
+        <v>19</v>
+      </c>
+      <c r="B20" s="7">
+        <v>139666</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="D20" s="7"/>
+      <c r="E20" s="16">
+        <v>9</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="6">
+        <v>20</v>
+      </c>
+      <c r="B21" s="20">
+        <v>141023</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>204</v>
+      </c>
+      <c r="E21" s="12">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="6">
+        <v>21</v>
+      </c>
+      <c r="B22" s="20">
+        <v>178684</v>
+      </c>
+      <c r="C22" s="20" t="s">
+        <v>206</v>
+      </c>
+      <c r="E22" s="12">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="6">
+        <v>22</v>
+      </c>
+      <c r="B23" s="20">
+        <v>187084</v>
+      </c>
+      <c r="C23" s="20" t="s">
+        <v>208</v>
+      </c>
+      <c r="E23" s="12">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="6">
+        <v>23</v>
+      </c>
+      <c r="B24" s="20">
+        <v>46013133</v>
+      </c>
+      <c r="C24" s="20" t="s">
+        <v>210</v>
+      </c>
+      <c r="E24" s="12">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="6">
+        <v>24</v>
+      </c>
+      <c r="B25" s="20">
+        <v>151158</v>
+      </c>
+      <c r="C25" s="20" t="s">
+        <v>212</v>
+      </c>
+      <c r="E25" s="12">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="6">
+        <v>25</v>
+      </c>
+      <c r="B26" s="20">
+        <v>142742</v>
+      </c>
+      <c r="C26" s="20" t="s">
+        <v>213</v>
+      </c>
+      <c r="D26" s="22" t="s">
+        <v>214</v>
+      </c>
+      <c r="E26" s="12"/>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="21">
+        <v>26</v>
+      </c>
+      <c r="B27" s="7">
+        <v>142584</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="E27" s="21"/>
+      <c r="F27" s="7"/>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="21">
+        <v>27</v>
+      </c>
+      <c r="B28" s="7">
+        <v>100578</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="E28" s="21"/>
+      <c r="F28" s="7"/>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="21">
+        <v>28</v>
+      </c>
+      <c r="B29" s="7">
+        <v>176569</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="E29" s="21"/>
+      <c r="F29" s="7"/>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="21">
+        <v>29</v>
+      </c>
+      <c r="B30" s="7">
+        <v>190871</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="E30" s="21"/>
+      <c r="F30" s="7"/>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="23">
+        <v>30</v>
+      </c>
+      <c r="B31" s="24">
+        <v>154223</v>
+      </c>
+      <c r="C31" s="24" t="s">
+        <v>220</v>
+      </c>
+      <c r="D31" s="24" t="s">
+        <v>221</v>
+      </c>
+      <c r="E31" s="24"/>
+      <c r="F31" s="24"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
@@ -21775,7 +22292,8 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -22000,7 +22518,8 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -22226,7 +22745,8 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
@@ -22486,7 +23006,8 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -22738,7 +23259,8 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
@@ -22987,7 +23509,8 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
@@ -23252,7 +23775,8 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Updated status for 21st & 22nd April
</commit_message>
<xml_diff>
--- a/CSD_Daily_status.xlsx
+++ b/CSD_Daily_status.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\bench_status\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prduhan\Documents\bench_status\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2849198F-573A-4FE7-8571-7F712D02630F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="17" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="18" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="status-18-03-2020" sheetId="14" r:id="rId1"/>
@@ -46,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1029" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1031" uniqueCount="233">
   <si>
     <t>Date</t>
   </si>
@@ -744,11 +743,14 @@
     <t>Going through Devops Training - Jenkins pipeline.
 2. attended interview for CIA, preparing for next round.</t>
   </si>
+  <si>
+    <t>Getting Product Data management training &amp; learning SQL</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1342,7 +1344,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD29"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
@@ -18087,7 +18089,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -18428,7 +18430,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -18775,7 +18777,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -19124,7 +19126,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -19476,7 +19478,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
@@ -19828,7 +19830,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -20180,7 +20182,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
@@ -20532,7 +20534,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -21103,10 +21105,10 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
@@ -21631,11 +21633,11 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B7C544D-9F63-4380-BC97-2CD68795D673}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23:D24"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -21862,7 +21864,7 @@
       </c>
       <c r="F13" s="12"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="14">
         <v>13</v>
       </c>
@@ -21871,6 +21873,9 @@
       </c>
       <c r="C14" s="27" t="s">
         <v>191</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>232</v>
       </c>
       <c r="E14" s="18">
         <v>9</v>
@@ -22139,7 +22144,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
@@ -22375,11 +22380,11 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56A65712-1E37-4785-81DF-4FB5C7685490}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -22606,7 +22611,7 @@
       </c>
       <c r="F13" s="12"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="14">
         <v>13</v>
       </c>
@@ -22615,6 +22620,9 @@
       </c>
       <c r="C14" s="27" t="s">
         <v>191</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>232</v>
       </c>
       <c r="E14" s="18">
         <v>9</v>
@@ -22883,7 +22891,7 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F076D7D1-4A44-4DF6-9EDC-8DD1D1068E68}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -23388,7 +23396,7 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45953738-7004-42F7-BFC2-4FD8F2577963}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -23893,7 +23901,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -24118,7 +24126,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -24344,7 +24352,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
@@ -24604,7 +24612,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -24856,7 +24864,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
@@ -25105,7 +25113,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
@@ -25370,7 +25378,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>